<commit_message>
Changes in nif example files
</commit_message>
<xml_diff>
--- a/src/gene_cluster_importer/data/part_attributes.xlsx
+++ b/src/gene_cluster_importer/data/part_attributes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="86">
   <si>
     <t>S0</t>
   </si>
@@ -268,13 +268,22 @@
   </si>
   <si>
     <t>Part</t>
+  </si>
+  <si>
+    <t>REU</t>
+  </si>
+  <si>
+    <t>REU_SD</t>
+  </si>
+  <si>
+    <t>Strength_SD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,11 +313,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,24 +336,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,7 +459,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Part Attributes'!$AO$2:$AO$105</c:f>
+              <c:f>'Part Attributes'!$AR$2:$AR$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="104"/>
@@ -441,7 +468,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Part Attributes'!$AN$2:$AN$105</c:f>
+              <c:f>'Part Attributes'!$AQ$2:$AQ$105</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="104"/>
@@ -458,11 +485,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2077321032"/>
-        <c:axId val="-2077254360"/>
+        <c:axId val="-2146118216"/>
+        <c:axId val="-2146210664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2077321032"/>
+        <c:axId val="-2146118216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -472,12 +499,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077254360"/>
+        <c:crossAx val="-2146210664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2077254360"/>
+        <c:axId val="-2146210664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077321032"/>
+        <c:crossAx val="-2146118216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -513,13 +540,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>38</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>43</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -831,388 +858,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="39" width="8.83203125" style="2"/>
-    <col min="40" max="40" width="29.1640625" style="2" customWidth="1"/>
-    <col min="41" max="41" width="30.83203125" style="2" customWidth="1"/>
-    <col min="42" max="42" width="11.83203125" style="2" customWidth="1"/>
-    <col min="43" max="43" width="11.1640625" style="2" customWidth="1"/>
-    <col min="44" max="44" width="15.6640625" style="2" customWidth="1"/>
-    <col min="45" max="45" width="13.1640625" style="2" customWidth="1"/>
-    <col min="46" max="46" width="14.5" style="2" customWidth="1"/>
-    <col min="47" max="47" width="12.5" style="2" customWidth="1"/>
-    <col min="48" max="48" width="12.83203125" style="2" customWidth="1"/>
-    <col min="49" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="42" width="8.83203125" style="1"/>
+    <col min="43" max="43" width="29.1640625" style="1" customWidth="1"/>
+    <col min="44" max="44" width="30.83203125" style="1" customWidth="1"/>
+    <col min="45" max="45" width="11.83203125" style="1" customWidth="1"/>
+    <col min="46" max="46" width="11.1640625" style="1" customWidth="1"/>
+    <col min="47" max="47" width="15.6640625" style="1" customWidth="1"/>
+    <col min="48" max="48" width="13.1640625" style="1" customWidth="1"/>
+    <col min="49" max="49" width="14.5" style="1" customWidth="1"/>
+    <col min="50" max="50" width="12.5" style="1" customWidth="1"/>
+    <col min="51" max="51" width="12.83203125" style="1" customWidth="1"/>
+    <col min="52" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="1">
+      <c r="E9" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="1">
+      <c r="E10" s="1">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="1">
+      <c r="E11" s="1">
         <v>0.121</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.77</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1">
+        <v>5.91</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.27</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="F17" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F21" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="F22" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -1222,91 +1316,87 @@
       <c r="C30" s="1">
         <v>2.62</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>